<commit_message>
Done with Single course selection
</commit_message>
<xml_diff>
--- a/data/Courses.xlsx
+++ b/data/Courses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\College Svce\Open-Elective\open-elective-service\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6F19FA5-CC28-455A-ACF3-5B588728FB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F25D172-48A3-4F8D-9E35-07D632FA554C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>